<commit_message>
update matrix for finance.
</commit_message>
<xml_diff>
--- a/ETLSystem - Finance/Finance_Bus_Matrix_v.1.xlsx
+++ b/ETLSystem - Finance/Finance_Bus_Matrix_v.1.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="240">
   <si>
     <t>Category</t>
   </si>
@@ -770,6 +770,9 @@
       </rPr>
       <t>(Question: some acounts will miss entity, debtor and costing,etc.)</t>
     </r>
+  </si>
+  <si>
+    <t>GLF_LDG_acct_desc1: do we need to filter based on LGD_NAME?</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1202,6 +1205,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5774,7 +5778,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="K13" sqref="K13:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6000,7 +6004,7 @@
       <c r="J13" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="K13" s="38" t="s">
+      <c r="K13" s="65" t="s">
         <v>238</v>
       </c>
     </row>
@@ -6029,7 +6033,9 @@
       <c r="J14" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="K14" s="38"/>
+      <c r="K14" s="65" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="15" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">

</xml_diff>

<commit_message>
added Matrix Bus folder for solution
</commit_message>
<xml_diff>
--- a/ETLSystem - Finance/Finance_Bus_Matrix_v.1.xlsx
+++ b/ETLSystem - Finance/Finance_Bus_Matrix_v.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="7050" windowWidth="24240" windowHeight="5925" firstSheet="18" activeTab="23"/>
+    <workbookView xWindow="-90" yWindow="7050" windowWidth="24240" windowHeight="5925" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Matrix" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="241">
   <si>
     <t>Category</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>GLF_LDG_acct_desc1: do we need to filter based on LGD_NAME?</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -4451,10 +4454,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4581,6 +4587,11 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4590,7 +4601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -5007,10 +5018,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5137,6 +5151,11 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5144,10 +5163,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5274,6 +5296,11 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5281,10 +5308,13 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5410,6 +5440,11 @@
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>240</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5777,7 +5812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K13" sqref="K13:K14"/>
     </sheetView>
   </sheetViews>
@@ -6716,10 +6751,13 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K10"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>